<commit_message>
Se agrega los script para tres market place adicionales.
Dkhardware, Edgesupply & PlumbingandElectric
</commit_message>
<xml_diff>
--- a/XX_Url/Gerber_URL.xlsx
+++ b/XX_Url/Gerber_URL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://orgcorona-my.sharepoint.com/personal/jmonsalvo_corona_com_co/Documents/03_Proy_ID/03_MACHINE_LEARNING/01_Projects/11_Web_Scrapping/Pricing/00_Sprint/00_Scrapping_code/XX_Url/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{ADD8D484-5C23-40E6-B751-62A63769F47D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA1A49BC-894F-4405-896C-8F31F231B44A}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{ADD8D484-5C23-40E6-B751-62A63769F47D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{11A3AEDE-9794-4FC8-B6D2-787CDD6A1298}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="URL" sheetId="2" r:id="rId1"/>
@@ -102,9 +102,6 @@
     <t>https://www.gerber-us.com/maxwell-1-6-gpf-12-rough-in-two-piece-elongated-toilet/products/us-GMX20912</t>
   </si>
   <si>
-    <t>GMX20918</t>
-  </si>
-  <si>
     <t>Maxwell® 1.28 gpf 12" Rough-In Two-Piece Elongated ErgoHeight™ Toilet</t>
   </si>
   <si>
@@ -187,6 +184,9 @@
   </si>
   <si>
     <t>Sku</t>
+  </si>
+  <si>
+    <t>GWS20918</t>
   </si>
 </sst>
 </file>
@@ -1134,7 +1134,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1153,13 +1153,13 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="C1" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -1171,10 +1171,10 @@
         <v>2</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>48</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>3</v>
@@ -1185,10 +1185,10 @@
     </row>
     <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>5</v>
@@ -1203,7 +1203,7 @@
         <v>7</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H2" s="4">
         <v>1.6</v>
@@ -1217,10 +1217,10 @@
     </row>
     <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>10</v>
@@ -1249,10 +1249,10 @@
     </row>
     <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>15</v>
@@ -1267,7 +1267,7 @@
         <v>17</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H4" s="4">
         <v>1.6</v>
@@ -1281,10 +1281,10 @@
     </row>
     <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>20</v>
@@ -1299,7 +1299,7 @@
         <v>17</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H5" s="4">
         <v>1.6</v>
@@ -1313,13 +1313,13 @@
     </row>
     <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>16</v>
@@ -1331,30 +1331,30 @@
         <v>7</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H6" s="4">
         <v>1.28</v>
       </c>
       <c r="I6" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" s="11" t="s">
         <v>24</v>
-      </c>
-      <c r="J6" s="11" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>27</v>
       </c>
       <c r="E7" s="6">
         <v>12</v>
@@ -1363,30 +1363,30 @@
         <v>17</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H7" s="4">
         <v>1.6</v>
       </c>
       <c r="I7" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" s="11" t="s">
         <v>28</v>
-      </c>
-      <c r="J7" s="11" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E8" s="6">
         <v>12</v>
@@ -1395,27 +1395,27 @@
         <v>7</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H8" s="4">
         <v>1.6</v>
       </c>
       <c r="I8" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" s="11" t="s">
         <v>31</v>
-      </c>
-      <c r="J8" s="11" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>16</v>
@@ -1427,16 +1427,16 @@
         <v>17</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H9" s="4">
         <v>1.28</v>
       </c>
       <c r="I9" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9" s="11" t="s">
         <v>34</v>
-      </c>
-      <c r="J9" s="11" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>